<commit_message>
pre-processing notebook for ammonia data
</commit_message>
<xml_diff>
--- a/code/input_data/fuels_HHV_industry_heat.xlsx
+++ b/code/input_data/fuels_HHV_industry_heat.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675B5480-05A9-4EB7-A0D5-70B22B6A67F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4BA1D3-522D-45C2-B16B-0800EC788271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{39A15509-65DE-424B-82F0-6774D28B4784}"/>
+    <workbookView xWindow="46140" yWindow="0" windowWidth="15390" windowHeight="9540" activeTab="2" xr2:uid="{39A15509-65DE-424B-82F0-6774D28B4784}"/>
   </bookViews>
   <sheets>
     <sheet name="fuel_map" sheetId="1" r:id="rId1"/>
     <sheet name="hhv" sheetId="2" r:id="rId2"/>
+    <sheet name="lhv" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="46">
   <si>
     <t>fuel</t>
   </si>
@@ -811,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F7F0246-8911-4C6D-9D2D-B1F4A1B708E8}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:AG1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -952,4 +953,134 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8CFE1C-3369-48C5-A78A-A6BA4D6E7E00}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="24.46484375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>47.140999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>42.790999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>43.448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>39.466000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>42.612000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8">
+        <v>22.731999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>26.122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>19.550999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>37.527999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>26.952000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>16.37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>46.898000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>